<commit_message>
Ensure consistency of naming convention
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_SUP_Hydrogen.xlsx
+++ b/SubRES_TMPL/SubRES_SUP_Hydrogen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56188274-7A1E-481C-AEA8-6209693E48D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FF47C25-6963-4D92-8624-78934334B8C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="48" r:id="rId1"/>
@@ -402,9 +402,6 @@
     <t>Hydrogen chain</t>
   </si>
   <si>
-    <t>ENV_ACT~Sink_SUPCO2N</t>
-  </si>
-  <si>
     <t>SUPH2GC</t>
   </si>
   <si>
@@ -468,6 +465,9 @@
   <si>
     <t>DAYNITE</t>
     <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>ENV_ACT~SUPCO2S</t>
   </si>
 </sst>
 </file>
@@ -1537,22 +1537,22 @@
       <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="8" width="14.1328125" style="4" customWidth="1"/>
-    <col min="9" max="9" width="12.1328125" style="4" customWidth="1"/>
-    <col min="10" max="12" width="8.1328125" style="4" customWidth="1"/>
-    <col min="13" max="13" width="9.6640625" style="4" customWidth="1"/>
-    <col min="14" max="14" width="8.1328125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="8" width="14.140625" style="4" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" style="4" customWidth="1"/>
+    <col min="10" max="12" width="8.140625" style="4" customWidth="1"/>
+    <col min="13" max="13" width="9.7109375" style="4" customWidth="1"/>
+    <col min="14" max="14" width="8.140625" style="4" customWidth="1"/>
     <col min="15" max="15" width="10" style="4" customWidth="1"/>
-    <col min="16" max="16" width="11.46484375" style="4" customWidth="1"/>
-    <col min="17" max="17" width="13.46484375" style="4" customWidth="1"/>
-    <col min="18" max="31" width="8.86328125" style="4"/>
-    <col min="32" max="32" width="21.46484375" style="4" customWidth="1"/>
-    <col min="33" max="38" width="8.86328125" style="4"/>
-    <col min="39" max="39" width="21.33203125" style="4" customWidth="1"/>
-    <col min="40" max="16384" width="8.86328125" style="4"/>
+    <col min="16" max="16" width="11.42578125" style="4" customWidth="1"/>
+    <col min="17" max="17" width="13.42578125" style="4" customWidth="1"/>
+    <col min="18" max="31" width="8.85546875" style="4"/>
+    <col min="32" max="32" width="21.42578125" style="4" customWidth="1"/>
+    <col min="33" max="38" width="8.85546875" style="4"/>
+    <col min="39" max="39" width="21.28515625" style="4" customWidth="1"/>
+    <col min="40" max="16384" width="8.85546875" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1974,33 +1974,33 @@
   </sheetPr>
   <dimension ref="A2:AE19"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="Q15" sqref="Q15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="33.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="56.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.1328125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="24.1328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="9.33203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="15.1328125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.6640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="17.1328125" style="1" customWidth="1"/>
-    <col min="10" max="19" width="11.1328125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="33.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="56.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="24.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="9.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="17.140625" style="1" customWidth="1"/>
+    <col min="10" max="19" width="11.140625" style="1" customWidth="1"/>
     <col min="20" max="21" width="12" style="1" customWidth="1"/>
-    <col min="22" max="22" width="8.86328125" style="2"/>
-    <col min="23" max="23" width="8.86328125" style="49"/>
-    <col min="24" max="24" width="13.6640625" style="2" customWidth="1"/>
+    <col min="22" max="22" width="8.85546875" style="2"/>
+    <col min="23" max="23" width="8.85546875" style="49"/>
+    <col min="24" max="24" width="13.7109375" style="2" customWidth="1"/>
     <col min="25" max="25" width="15" style="2" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="68.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="27" max="16384" width="8.86328125" style="2"/>
+    <col min="26" max="26" width="68.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="27" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:31" s="49" customFormat="1" ht="23.25">
       <c r="A2" s="16" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B2" s="17"/>
       <c r="C2" s="48"/>
@@ -2083,7 +2083,7 @@
       <c r="AD4" s="34"/>
       <c r="AE4" s="23"/>
     </row>
-    <row r="5" spans="1:31" s="49" customFormat="1" ht="26.25">
+    <row r="5" spans="1:31" s="49" customFormat="1" ht="25.5">
       <c r="A5" s="32" t="s">
         <v>1</v>
       </c>
@@ -2142,7 +2142,7 @@
         <v>32</v>
       </c>
       <c r="T5" s="32" t="s">
-        <v>118</v>
+        <v>139</v>
       </c>
       <c r="U5" s="32" t="s">
         <v>87</v>
@@ -2172,7 +2172,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="6" spans="1:31" s="49" customFormat="1" ht="79.150000000000006" thickBot="1">
+    <row r="6" spans="1:31" s="49" customFormat="1" ht="77.25" thickBot="1">
       <c r="A6" s="19" t="s">
         <v>11</v>
       </c>
@@ -2318,16 +2318,16 @@
     </row>
     <row r="9" spans="1:31" s="49" customFormat="1">
       <c r="A9" s="48" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B9" s="49" t="s">
         <v>82</v>
       </c>
       <c r="C9" s="48" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D9" s="49" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E9" s="48">
         <v>2013</v>
@@ -2417,15 +2417,6 @@
       <c r="O10" s="48"/>
       <c r="P10" s="48"/>
       <c r="Q10" s="48"/>
-      <c r="S10" s="37" t="s">
-        <v>91</v>
-      </c>
-      <c r="T10" s="37">
-        <v>96.1</v>
-      </c>
-      <c r="U10" s="37">
-        <v>0.9</v>
-      </c>
       <c r="V10" s="48"/>
       <c r="W10" s="48"/>
     </row>
@@ -2447,13 +2438,13 @@
       <c r="P11" s="48"/>
       <c r="Q11" s="48"/>
       <c r="S11" s="37" t="s">
-        <v>92</v>
-      </c>
-      <c r="T11" s="38">
-        <v>75.3</v>
-      </c>
-      <c r="U11" s="38">
-        <v>0.88</v>
+        <v>91</v>
+      </c>
+      <c r="T11" s="37">
+        <v>96.1</v>
+      </c>
+      <c r="U11" s="37">
+        <v>0.9</v>
       </c>
       <c r="V11" s="48" t="s">
         <v>94</v>
@@ -2478,13 +2469,13 @@
       <c r="P12" s="48"/>
       <c r="Q12" s="48"/>
       <c r="S12" s="37" t="s">
-        <v>93</v>
-      </c>
-      <c r="T12" s="37">
-        <v>56.1</v>
-      </c>
-      <c r="U12" s="37">
-        <v>0.95</v>
+        <v>92</v>
+      </c>
+      <c r="T12" s="38">
+        <v>75.3</v>
+      </c>
+      <c r="U12" s="38">
+        <v>0.88</v>
       </c>
       <c r="V12" s="48"/>
       <c r="W12" s="48"/>
@@ -2506,15 +2497,21 @@
       <c r="O13" s="48"/>
       <c r="P13" s="48"/>
       <c r="Q13" s="48"/>
-      <c r="S13" s="37"/>
-      <c r="T13" s="37"/>
-      <c r="U13" s="37"/>
+      <c r="S13" s="37" t="s">
+        <v>93</v>
+      </c>
+      <c r="T13" s="37">
+        <v>56.1</v>
+      </c>
+      <c r="U13" s="37">
+        <v>0.95</v>
+      </c>
       <c r="V13" s="48"/>
       <c r="W13" s="48"/>
     </row>
     <row r="14" spans="1:31" s="49" customFormat="1" ht="23.25">
       <c r="A14" s="16" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B14" s="17"/>
       <c r="C14" s="47"/>
@@ -2606,7 +2603,7 @@
       <c r="AD16" s="34"/>
       <c r="AE16" s="23"/>
     </row>
-    <row r="17" spans="1:31" s="49" customFormat="1" ht="26.25">
+    <row r="17" spans="1:31" s="49" customFormat="1" ht="25.5">
       <c r="A17" s="41" t="s">
         <v>1</v>
       </c>
@@ -2635,7 +2632,7 @@
         <v>10</v>
       </c>
       <c r="J17" s="42" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K17" s="42" t="s">
         <v>25</v>
@@ -2644,16 +2641,16 @@
         <v>27</v>
       </c>
       <c r="M17" s="42" t="s">
+        <v>123</v>
+      </c>
+      <c r="N17" s="42" t="s">
         <v>124</v>
       </c>
-      <c r="N17" s="42" t="s">
+      <c r="O17" s="42" t="s">
         <v>125</v>
       </c>
-      <c r="O17" s="42" t="s">
+      <c r="P17" s="42" t="s">
         <v>126</v>
-      </c>
-      <c r="P17" s="42" t="s">
-        <v>127</v>
       </c>
       <c r="Q17" s="47"/>
       <c r="R17" s="48"/>
@@ -2685,7 +2682,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="18" spans="1:31" s="49" customFormat="1" ht="14.65" thickBot="1">
+    <row r="18" spans="1:31" s="49" customFormat="1" ht="15.75" thickBot="1">
       <c r="A18" s="44" t="s">
         <v>11</v>
       </c>
@@ -2700,7 +2697,7 @@
       </c>
       <c r="E18" s="44"/>
       <c r="F18" s="44" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G18" s="44" t="s">
         <v>20</v>
@@ -2709,11 +2706,11 @@
       <c r="I18" s="44"/>
       <c r="J18" s="44"/>
       <c r="K18" s="44" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L18" s="44"/>
       <c r="M18" s="44" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="N18" s="44"/>
       <c r="O18" s="44" t="s">
@@ -2738,16 +2735,16 @@
     </row>
     <row r="19" spans="1:31" s="49" customFormat="1">
       <c r="A19" s="48" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B19" s="49" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C19" s="49" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D19" s="49" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E19" s="49">
         <v>1</v>
@@ -2818,23 +2815,23 @@
   <dimension ref="A1:Y10"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="29.33203125" style="1" customWidth="1"/>
-    <col min="3" max="5" width="12.86328125" style="1" customWidth="1"/>
-    <col min="6" max="7" width="8.86328125" style="1"/>
-    <col min="8" max="8" width="13.86328125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="8.86328125" style="1"/>
-    <col min="10" max="16" width="16.6640625" style="1" customWidth="1"/>
-    <col min="17" max="17" width="8.86328125" style="1"/>
-    <col min="18" max="18" width="11.6640625" style="1" customWidth="1"/>
-    <col min="19" max="19" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="29.28515625" style="1" customWidth="1"/>
+    <col min="3" max="5" width="12.85546875" style="1" customWidth="1"/>
+    <col min="6" max="7" width="8.85546875" style="1"/>
+    <col min="8" max="8" width="13.85546875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="8.85546875" style="1"/>
+    <col min="10" max="16" width="16.7109375" style="1" customWidth="1"/>
+    <col min="17" max="17" width="8.85546875" style="1"/>
+    <col min="18" max="18" width="11.7109375" style="1" customWidth="1"/>
+    <col min="19" max="19" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="16384" width="8.86328125" style="1"/>
+    <col min="21" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="23.25">
@@ -2936,7 +2933,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="92.25" thickBot="1">
+    <row r="5" spans="1:25" ht="90" thickBot="1">
       <c r="A5" s="19" t="s">
         <v>11</v>
       </c>
@@ -3079,7 +3076,7 @@
         <v>96</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F8" s="1">
         <v>2013</v>
@@ -3143,7 +3140,7 @@
         <v>41</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="10" spans="1:25">
@@ -3175,19 +3172,19 @@
   <dimension ref="A1:AA14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15" style="1" customWidth="1"/>
-    <col min="2" max="2" width="57.46484375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="12.53125" style="1" customWidth="1"/>
-    <col min="5" max="18" width="14.33203125" style="1" customWidth="1"/>
-    <col min="19" max="20" width="8.86328125" style="1"/>
-    <col min="21" max="21" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="56.53125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="8.86328125" style="1"/>
+    <col min="2" max="2" width="57.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.5703125" style="1" customWidth="1"/>
+    <col min="5" max="18" width="14.28515625" style="1" customWidth="1"/>
+    <col min="19" max="20" width="8.85546875" style="1"/>
+    <col min="21" max="21" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="56.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="23.25">
@@ -3215,7 +3212,7 @@
       <c r="Y3" s="34"/>
       <c r="Z3" s="34"/>
     </row>
-    <row r="4" spans="1:27">
+    <row r="4" spans="1:27" ht="25.5">
       <c r="A4" s="32" t="s">
         <v>1</v>
       </c>
@@ -3295,7 +3292,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="1:27" ht="92.25" thickBot="1">
+    <row r="5" spans="1:27" ht="102.75" thickBot="1">
       <c r="A5" s="19" t="s">
         <v>11</v>
       </c>
@@ -3454,10 +3451,10 @@
         <v>102</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E8" s="1">
         <v>2013</v>
@@ -3526,10 +3523,10 @@
         <v>103</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E9" s="1">
         <v>2013</v>
@@ -3596,10 +3593,10 @@
         <v>104</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E10" s="1">
         <v>2013</v>
@@ -3686,28 +3683,28 @@
   </sheetPr>
   <dimension ref="A1:W9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="S8" sqref="S8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="24.46484375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="10.46484375" style="1" customWidth="1"/>
-    <col min="5" max="6" width="8.86328125" style="1"/>
-    <col min="7" max="7" width="14.53125" style="1" customWidth="1"/>
-    <col min="8" max="9" width="8.86328125" style="1"/>
-    <col min="10" max="10" width="14.53125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.6640625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="6.53125" customWidth="1"/>
-    <col min="14" max="14" width="11.53125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.86328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="23.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="22" width="8.86328125" style="1"/>
-    <col min="23" max="23" width="2.6640625" customWidth="1"/>
-    <col min="24" max="16384" width="8.86328125" style="1"/>
+    <col min="1" max="1" width="17.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.42578125" style="1" customWidth="1"/>
+    <col min="5" max="6" width="8.85546875" style="1"/>
+    <col min="7" max="7" width="14.5703125" style="1" customWidth="1"/>
+    <col min="8" max="9" width="8.85546875" style="1"/>
+    <col min="10" max="10" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" style="1" customWidth="1"/>
+    <col min="13" max="13" width="6.5703125" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="23.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="22" width="8.85546875" style="1"/>
+    <col min="23" max="23" width="2.7109375" customWidth="1"/>
+    <col min="24" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25">
@@ -3887,10 +3884,10 @@
         <v>115</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E7" s="1">
         <v>2013</v>
@@ -3934,10 +3931,10 @@
         <v>88</v>
       </c>
       <c r="S7" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="U7" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="8" spans="1:21">
@@ -3948,10 +3945,10 @@
         <v>116</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E8" s="2">
         <v>2013</v>
@@ -3992,10 +3989,10 @@
         <v>88</v>
       </c>
       <c r="S8" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="U8" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="9" spans="1:21">
@@ -4011,18 +4008,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4205,18 +4202,18 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E5D25AEF-5EEE-4730-89DA-F522B2580678}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C84C340F-40A4-4836-8E7A-67ECA799FFAF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C84C340F-40A4-4836-8E7A-67ECA799FFAF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E5D25AEF-5EEE-4730-89DA-F522B2580678}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Most new technologies can start from 2019
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_SUP_Hydrogen.xlsx
+++ b/SubRES_TMPL/SubRES_SUP_Hydrogen.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F1D8ACB5-1DDB-4630-95B7-47ECCE9435F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A15BABD-44E3-424B-8FC9-8267CFE6931F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{62F67F8D-DFD4-4ADE-8356-63F780461C4E}"/>
+    <workbookView xWindow="-3233" yWindow="8002" windowWidth="20716" windowHeight="13276" activeTab="2" xr2:uid="{62F67F8D-DFD4-4ADE-8356-63F780461C4E}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="2" r:id="rId1"/>
@@ -734,10 +734,6 @@
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
@@ -747,10 +743,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -772,10 +764,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -830,6 +818,18 @@
     <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1436,98 +1436,98 @@
       <c r="F16" s="2"/>
     </row>
     <row r="17" spans="1:14" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="17" t="s">
+      <c r="A17" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="16"/>
-      <c r="H17" s="16"/>
-      <c r="I17" s="15"/>
-      <c r="J17" s="15"/>
-      <c r="K17" s="15"/>
-      <c r="L17" s="15"/>
-      <c r="M17" s="15"/>
-      <c r="N17" s="15"/>
+      <c r="B17" s="38"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="13"/>
+      <c r="M17" s="13"/>
+      <c r="N17" s="13"/>
     </row>
     <row r="18" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="14"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
+      <c r="A18" s="12"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
     </row>
     <row r="19" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="14"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="13"/>
-      <c r="I19" s="12"/>
-      <c r="J19" s="12"/>
-      <c r="K19" s="12"/>
-      <c r="L19" s="12"/>
-      <c r="M19" s="12"/>
-      <c r="N19" s="12"/>
+      <c r="A19" s="12"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="10"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="10"/>
+      <c r="M19" s="10"/>
+      <c r="N19" s="10"/>
     </row>
     <row r="20" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="s">
+      <c r="A20" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="10"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="9"/>
-      <c r="K20" s="9"/>
-      <c r="L20" s="9"/>
-      <c r="M20" s="9"/>
-      <c r="N20" s="9"/>
+      <c r="C20" s="39"/>
+      <c r="D20" s="39"/>
+      <c r="E20" s="39"/>
+      <c r="F20" s="39"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="8"/>
+      <c r="L20" s="8"/>
+      <c r="M20" s="8"/>
+      <c r="N20" s="8"/>
     </row>
     <row r="21" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="8" t="s">
+      <c r="A21" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B21" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="10"/>
-      <c r="I21" s="9"/>
-      <c r="J21" s="9"/>
-      <c r="K21" s="9"/>
-      <c r="L21" s="9"/>
-      <c r="M21" s="9"/>
-      <c r="N21" s="9"/>
+      <c r="C21" s="40"/>
+      <c r="D21" s="40"/>
+      <c r="E21" s="40"/>
+      <c r="F21" s="40"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="8"/>
+      <c r="L21" s="8"/>
+      <c r="M21" s="8"/>
+      <c r="N21" s="8"/>
     </row>
     <row r="22" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="s">
+      <c r="A22" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="B22" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
+      <c r="C22" s="40"/>
+      <c r="D22" s="40"/>
+      <c r="E22" s="40"/>
+      <c r="F22" s="40"/>
     </row>
     <row r="23" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
@@ -1725,381 +1725,381 @@
   </sheetPr>
   <dimension ref="A2:AE17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.7109375" style="18" customWidth="1"/>
-    <col min="2" max="2" width="56.7109375" style="18" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" style="18" customWidth="1"/>
-    <col min="4" max="4" width="24.140625" style="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="9.28515625" style="18" customWidth="1"/>
-    <col min="7" max="7" width="15.140625" style="18" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" style="18" customWidth="1"/>
-    <col min="9" max="9" width="17.140625" style="18" customWidth="1"/>
-    <col min="10" max="19" width="11.140625" style="18" customWidth="1"/>
-    <col min="20" max="21" width="12" style="18" customWidth="1"/>
-    <col min="22" max="23" width="8.85546875" style="18"/>
-    <col min="24" max="24" width="13.7109375" style="18" customWidth="1"/>
-    <col min="25" max="25" width="15" style="18" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="68.7109375" style="18" bestFit="1" customWidth="1"/>
-    <col min="27" max="16384" width="8.85546875" style="18"/>
+    <col min="1" max="1" width="33.7109375" style="15" customWidth="1"/>
+    <col min="2" max="2" width="56.7109375" style="15" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" style="15" customWidth="1"/>
+    <col min="4" max="4" width="24.140625" style="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="9.28515625" style="15" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" style="15" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" style="15" customWidth="1"/>
+    <col min="9" max="9" width="17.140625" style="15" customWidth="1"/>
+    <col min="10" max="19" width="11.140625" style="15" customWidth="1"/>
+    <col min="20" max="21" width="12" style="15" customWidth="1"/>
+    <col min="22" max="23" width="8.85546875" style="15"/>
+    <col min="24" max="24" width="13.7109375" style="15" customWidth="1"/>
+    <col min="25" max="25" width="15" style="15" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="68.7109375" style="15" bestFit="1" customWidth="1"/>
+    <col min="27" max="16384" width="8.85546875" style="15"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:31" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="B2" s="28"/>
+      <c r="B2" s="25"/>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="24"/>
+      <c r="B3" s="21"/>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A4" s="24"/>
-      <c r="B4" s="24"/>
-      <c r="D4" s="26" t="s">
+      <c r="A4" s="21"/>
+      <c r="B4" s="21"/>
+      <c r="D4" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="X4" s="26" t="s">
+      <c r="X4" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="Y4" s="25"/>
-      <c r="Z4" s="25"/>
-      <c r="AA4" s="25"/>
-      <c r="AB4" s="25"/>
-      <c r="AC4" s="25"/>
-      <c r="AD4" s="25"/>
-      <c r="AE4" s="24"/>
+      <c r="Y4" s="22"/>
+      <c r="Z4" s="22"/>
+      <c r="AA4" s="22"/>
+      <c r="AB4" s="22"/>
+      <c r="AC4" s="22"/>
+      <c r="AD4" s="22"/>
+      <c r="AE4" s="21"/>
     </row>
     <row r="5" spans="1:31" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="38" t="s">
+      <c r="B5" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="C5" s="38" t="s">
+      <c r="C5" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="D5" s="38" t="s">
+      <c r="D5" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="E5" s="38" t="s">
+      <c r="E5" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="F5" s="38" t="s">
+      <c r="F5" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="G5" s="38" t="s">
+      <c r="G5" s="35" t="s">
         <v>84</v>
       </c>
-      <c r="H5" s="38" t="s">
+      <c r="H5" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="I5" s="38" t="s">
+      <c r="I5" s="35" t="s">
         <v>83</v>
       </c>
-      <c r="J5" s="38" t="s">
+      <c r="J5" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="K5" s="38" t="s">
+      <c r="K5" s="35" t="s">
         <v>82</v>
       </c>
-      <c r="L5" s="38" t="s">
+      <c r="L5" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="M5" s="38" t="s">
+      <c r="M5" s="35" t="s">
         <v>81</v>
       </c>
-      <c r="N5" s="38" t="s">
+      <c r="N5" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="O5" s="38" t="s">
+      <c r="O5" s="35" t="s">
         <v>80</v>
       </c>
-      <c r="P5" s="38" t="s">
+      <c r="P5" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="Q5" s="38" t="s">
+      <c r="Q5" s="35" t="s">
         <v>78</v>
       </c>
-      <c r="R5" s="38" t="s">
+      <c r="R5" s="35" t="s">
         <v>77</v>
       </c>
-      <c r="S5" s="38" t="s">
+      <c r="S5" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="T5" s="38" t="s">
+      <c r="T5" s="35" t="s">
         <v>75</v>
       </c>
-      <c r="U5" s="38" t="s">
+      <c r="U5" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="X5" s="21" t="s">
+      <c r="X5" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="Y5" s="21" t="s">
+      <c r="Y5" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="Z5" s="21" t="s">
+      <c r="Z5" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="AA5" s="21" t="s">
+      <c r="AA5" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="AB5" s="21" t="s">
+      <c r="AB5" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="AC5" s="21" t="s">
+      <c r="AC5" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="AD5" s="21" t="s">
+      <c r="AD5" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="AE5" s="21" t="s">
+      <c r="AE5" s="18" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:31" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="36" t="s">
+      <c r="A6" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="36" t="s">
+      <c r="C6" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="36" t="s">
+      <c r="D6" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="E6" s="36"/>
-      <c r="F6" s="36" t="s">
+      <c r="E6" s="33"/>
+      <c r="F6" s="33" t="s">
         <v>73</v>
       </c>
-      <c r="G6" s="36" t="s">
+      <c r="G6" s="33" t="s">
         <v>72</v>
       </c>
-      <c r="H6" s="36" t="s">
+      <c r="H6" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="I6" s="36" t="s">
+      <c r="I6" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="J6" s="36" t="s">
+      <c r="J6" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="K6" s="36" t="s">
+      <c r="K6" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="L6" s="37" t="s">
+      <c r="L6" s="34" t="s">
         <v>67</v>
       </c>
-      <c r="M6" s="36"/>
-      <c r="N6" s="36"/>
-      <c r="O6" s="36"/>
-      <c r="P6" s="37" t="s">
+      <c r="M6" s="33"/>
+      <c r="N6" s="33"/>
+      <c r="O6" s="33"/>
+      <c r="P6" s="34" t="s">
         <v>66</v>
       </c>
-      <c r="Q6" s="36"/>
-      <c r="R6" s="36"/>
-      <c r="S6" s="36"/>
-      <c r="T6" s="37" t="s">
+      <c r="Q6" s="33"/>
+      <c r="R6" s="33"/>
+      <c r="S6" s="33"/>
+      <c r="T6" s="34" t="s">
         <v>65</v>
       </c>
-      <c r="U6" s="36"/>
-      <c r="X6" s="35" t="s">
+      <c r="U6" s="33"/>
+      <c r="X6" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="Y6" s="35"/>
-      <c r="Z6" s="35"/>
-      <c r="AA6" s="35"/>
-      <c r="AB6" s="35"/>
-      <c r="AC6" s="35"/>
-      <c r="AD6" s="35"/>
-      <c r="AE6" s="35"/>
+      <c r="Y6" s="32"/>
+      <c r="Z6" s="32"/>
+      <c r="AA6" s="32"/>
+      <c r="AB6" s="32"/>
+      <c r="AC6" s="32"/>
+      <c r="AD6" s="32"/>
+      <c r="AE6" s="32"/>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A7" s="33" t="s">
+      <c r="A7" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="B7" s="33"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33" t="s">
+      <c r="B7" s="30"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="33" t="s">
+      <c r="F7" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="G7" s="33" t="s">
+      <c r="G7" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="H7" s="33"/>
-      <c r="I7" s="33" t="s">
+      <c r="H7" s="30"/>
+      <c r="I7" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="J7" s="33"/>
-      <c r="K7" s="33"/>
-      <c r="L7" s="34" t="s">
+      <c r="J7" s="30"/>
+      <c r="K7" s="30"/>
+      <c r="L7" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="M7" s="33"/>
-      <c r="N7" s="33"/>
-      <c r="O7" s="33"/>
-      <c r="P7" s="34" t="s">
+      <c r="M7" s="30"/>
+      <c r="N7" s="30"/>
+      <c r="O7" s="30"/>
+      <c r="P7" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="Q7" s="33"/>
-      <c r="R7" s="33"/>
-      <c r="S7" s="33"/>
-      <c r="T7" s="33" t="s">
+      <c r="Q7" s="30"/>
+      <c r="R7" s="30"/>
+      <c r="S7" s="30"/>
+      <c r="T7" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="U7" s="33"/>
-      <c r="X7" s="33" t="s">
+      <c r="U7" s="30"/>
+      <c r="X7" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="Y7" s="33"/>
-      <c r="Z7" s="33"/>
-      <c r="AA7" s="33"/>
-      <c r="AB7" s="33"/>
-      <c r="AC7" s="33"/>
-      <c r="AD7" s="33"/>
-      <c r="AE7" s="33"/>
+      <c r="Y7" s="30"/>
+      <c r="Z7" s="30"/>
+      <c r="AA7" s="30"/>
+      <c r="AB7" s="30"/>
+      <c r="AC7" s="30"/>
+      <c r="AD7" s="30"/>
+      <c r="AE7" s="30"/>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A8" s="30" t="s">
+      <c r="A8" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="B8" s="31"/>
-      <c r="C8" s="31"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="31"/>
-      <c r="G8" s="31"/>
-      <c r="H8" s="31"/>
-      <c r="I8" s="31"/>
-      <c r="J8" s="31"/>
-      <c r="K8" s="31"/>
-      <c r="L8" s="32"/>
-      <c r="M8" s="32"/>
-      <c r="N8" s="32"/>
-      <c r="O8" s="32"/>
-      <c r="P8" s="32"/>
-      <c r="Q8" s="32"/>
-      <c r="R8" s="32"/>
-      <c r="S8" s="32"/>
-      <c r="T8" s="31"/>
-      <c r="U8" s="31"/>
-      <c r="X8" s="30" t="str">
+      <c r="B8" s="28"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="28"/>
+      <c r="J8" s="28"/>
+      <c r="K8" s="28"/>
+      <c r="L8" s="29"/>
+      <c r="M8" s="29"/>
+      <c r="N8" s="29"/>
+      <c r="O8" s="29"/>
+      <c r="P8" s="29"/>
+      <c r="Q8" s="29"/>
+      <c r="R8" s="29"/>
+      <c r="S8" s="29"/>
+      <c r="T8" s="28"/>
+      <c r="U8" s="28"/>
+      <c r="X8" s="27" t="str">
         <f>A8</f>
         <v>* Electrolysis</v>
       </c>
-      <c r="Y8" s="30"/>
-      <c r="Z8" s="30"/>
-      <c r="AA8" s="30"/>
-      <c r="AB8" s="30"/>
-      <c r="AC8" s="30"/>
-      <c r="AD8" s="30"/>
-      <c r="AE8" s="30"/>
+      <c r="Y8" s="27"/>
+      <c r="Z8" s="27"/>
+      <c r="AA8" s="27"/>
+      <c r="AB8" s="27"/>
+      <c r="AC8" s="27"/>
+      <c r="AD8" s="27"/>
+      <c r="AE8" s="27"/>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="D9" s="18" t="s">
+      <c r="D9" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="E9" s="18">
-        <v>2013</v>
-      </c>
-      <c r="F9" s="18">
+      <c r="E9" s="15">
+        <v>2019</v>
+      </c>
+      <c r="F9" s="15">
         <v>30</v>
       </c>
-      <c r="G9" s="18">
+      <c r="G9" s="15">
         <v>-2</v>
       </c>
-      <c r="H9" s="18">
+      <c r="H9" s="15">
         <v>1</v>
       </c>
-      <c r="I9" s="18">
+      <c r="I9" s="15">
         <v>0.9</v>
       </c>
-      <c r="J9" s="18">
+      <c r="J9" s="15">
         <v>0.75</v>
       </c>
-      <c r="K9" s="18">
+      <c r="K9" s="15">
         <v>0.9</v>
       </c>
-      <c r="L9" s="19">
+      <c r="L9" s="16">
         <v>33.031619153587783</v>
       </c>
-      <c r="M9" s="19">
+      <c r="M9" s="16">
         <v>18.350899529770992</v>
       </c>
-      <c r="N9" s="19">
+      <c r="N9" s="16">
         <v>18.350899529770992</v>
       </c>
-      <c r="O9" s="19">
+      <c r="O9" s="16">
         <v>18.350899529770992</v>
       </c>
-      <c r="P9" s="19">
+      <c r="P9" s="16">
         <v>1.6515809576793894</v>
       </c>
-      <c r="Q9" s="19">
+      <c r="Q9" s="16">
         <v>0.9175449764885496</v>
       </c>
-      <c r="R9" s="19"/>
-      <c r="S9" s="19"/>
-      <c r="X9" s="18" t="s">
+      <c r="R9" s="16"/>
+      <c r="S9" s="16"/>
+      <c r="X9" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="Y9" s="18" t="str">
+      <c r="Y9" s="15" t="str">
         <f>A9</f>
         <v>SH2PCELC_01</v>
       </c>
-      <c r="Z9" s="18" t="str">
+      <c r="Z9" s="15" t="str">
         <f>B9</f>
         <v>Hydrogen production - Centralized Electrolysis</v>
       </c>
-      <c r="AA9" s="18" t="s">
+      <c r="AA9" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="AB9" s="18" t="s">
+      <c r="AB9" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="AC9" s="18" t="s">
+      <c r="AC9" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="AD9" s="18" t="s">
+      <c r="AD9" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="AE9" s="18" t="s">
+      <c r="AE9" s="15" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="L10" s="19"/>
-      <c r="M10" s="19"/>
-      <c r="N10" s="19"/>
-      <c r="O10" s="19"/>
-      <c r="P10" s="19"/>
-      <c r="Q10" s="19"/>
-      <c r="R10" s="19"/>
-      <c r="S10" s="19"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="16"/>
+      <c r="N10" s="16"/>
+      <c r="O10" s="16"/>
+      <c r="P10" s="16"/>
+      <c r="Q10" s="16"/>
+      <c r="R10" s="16"/>
+      <c r="S10" s="16"/>
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="S11"/>
@@ -2107,10 +2107,10 @@
       <c r="U11"/>
     </row>
     <row r="12" spans="1:31" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A12" s="29" t="s">
+      <c r="A12" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="B12" s="28"/>
+      <c r="B12" s="25"/>
       <c r="C12"/>
       <c r="D12"/>
       <c r="E12"/>
@@ -2137,12 +2137,12 @@
       <c r="Z12"/>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A13" s="24" t="s">
+      <c r="A13" s="21" t="s">
         <v>53</v>
       </c>
       <c r="B13"/>
       <c r="C13"/>
-      <c r="D13" s="24"/>
+      <c r="D13" s="21"/>
       <c r="E13"/>
       <c r="F13"/>
       <c r="G13"/>
@@ -2167,9 +2167,9 @@
       <c r="Z13"/>
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A14" s="27"/>
+      <c r="A14" s="24"/>
       <c r="C14"/>
-      <c r="D14" s="26" t="s">
+      <c r="D14" s="23" t="s">
         <v>52</v>
       </c>
       <c r="E14"/>
@@ -2185,199 +2185,199 @@
       <c r="O14"/>
       <c r="P14"/>
       <c r="Q14"/>
-      <c r="X14" s="26" t="s">
+      <c r="X14" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="Y14" s="25"/>
-      <c r="Z14" s="25"/>
-      <c r="AA14" s="25"/>
-      <c r="AB14" s="25"/>
-      <c r="AC14" s="25"/>
-      <c r="AD14" s="25"/>
-      <c r="AE14" s="24"/>
+      <c r="Y14" s="22"/>
+      <c r="Z14" s="22"/>
+      <c r="AA14" s="22"/>
+      <c r="AB14" s="22"/>
+      <c r="AC14" s="22"/>
+      <c r="AD14" s="22"/>
+      <c r="AE14" s="21"/>
     </row>
     <row r="15" spans="1:31" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="23" t="s">
+      <c r="A15" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="23" t="s">
+      <c r="B15" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="C15" s="23" t="s">
+      <c r="C15" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="D15" s="23" t="s">
+      <c r="D15" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="E15" s="22" t="s">
+      <c r="E15" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="F15" s="22" t="s">
+      <c r="F15" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="G15" s="22" t="s">
+      <c r="G15" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="H15" s="22" t="s">
+      <c r="H15" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="I15" s="22" t="s">
+      <c r="I15" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="J15" s="22" t="s">
+      <c r="J15" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="K15" s="22" t="s">
+      <c r="K15" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="L15" s="22" t="s">
+      <c r="L15" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="M15" s="22" t="s">
+      <c r="M15" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="N15" s="22" t="s">
+      <c r="N15" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="O15" s="22" t="s">
+      <c r="O15" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="P15" s="22" t="s">
+      <c r="P15" s="19" t="s">
         <v>36</v>
       </c>
       <c r="Q15"/>
-      <c r="X15" s="21" t="s">
+      <c r="X15" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="Y15" s="21" t="s">
+      <c r="Y15" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="Z15" s="21" t="s">
+      <c r="Z15" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="AA15" s="21" t="s">
+      <c r="AA15" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="AB15" s="21" t="s">
+      <c r="AB15" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="AC15" s="21" t="s">
+      <c r="AC15" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="AD15" s="21" t="s">
+      <c r="AD15" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="AE15" s="21" t="s">
+      <c r="AE15" s="18" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="20" t="s">
+      <c r="A16" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="20" t="s">
+      <c r="C16" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="20" t="s">
+      <c r="D16" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="E16" s="20"/>
-      <c r="F16" s="20" t="s">
+      <c r="E16" s="17"/>
+      <c r="F16" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="G16" s="20" t="s">
+      <c r="G16" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="H16" s="20"/>
-      <c r="I16" s="20"/>
-      <c r="J16" s="20"/>
-      <c r="K16" s="20" t="s">
+      <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="17"/>
+      <c r="K16" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="L16" s="20"/>
-      <c r="M16" s="20" t="s">
+      <c r="L16" s="17"/>
+      <c r="M16" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="N16" s="20"/>
-      <c r="O16" s="20" t="s">
+      <c r="N16" s="17"/>
+      <c r="O16" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="P16" s="20"/>
+      <c r="P16" s="17"/>
       <c r="Q16"/>
-      <c r="X16" s="20" t="s">
+      <c r="X16" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="Y16" s="20"/>
-      <c r="Z16" s="20"/>
-      <c r="AA16" s="20"/>
-      <c r="AB16" s="20"/>
-      <c r="AC16" s="20"/>
-      <c r="AD16" s="20"/>
-      <c r="AE16" s="20"/>
+      <c r="Y16" s="17"/>
+      <c r="Z16" s="17"/>
+      <c r="AA16" s="17"/>
+      <c r="AB16" s="17"/>
+      <c r="AC16" s="17"/>
+      <c r="AD16" s="17"/>
+      <c r="AE16" s="17"/>
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A17" s="18" t="s">
+      <c r="A17" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="18" t="s">
+      <c r="B17" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="18" t="s">
+      <c r="C17" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="18" t="s">
+      <c r="D17" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="E17" s="18">
+      <c r="E17" s="15">
         <v>1</v>
       </c>
-      <c r="F17" s="18">
-        <v>2013</v>
-      </c>
-      <c r="G17" s="18">
+      <c r="F17" s="15">
+        <v>2019</v>
+      </c>
+      <c r="G17" s="15">
         <v>20</v>
       </c>
-      <c r="H17" s="18">
+      <c r="H17" s="15">
         <v>0.95</v>
       </c>
-      <c r="I17" s="18">
+      <c r="I17" s="15">
         <v>0.75</v>
       </c>
-      <c r="J17" s="18">
+      <c r="J17" s="15">
         <v>0.85</v>
       </c>
-      <c r="K17" s="19">
+      <c r="K17" s="16">
         <v>79.340256372000013</v>
       </c>
-      <c r="L17" s="19">
+      <c r="L17" s="16">
         <v>19.529909260800004</v>
       </c>
       <c r="Q17"/>
-      <c r="X17" s="18" t="s">
+      <c r="X17" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="Y17" s="18" t="str">
+      <c r="Y17" s="15" t="str">
         <f>A17</f>
         <v>SH2PDELC_01</v>
       </c>
-      <c r="Z17" s="18" t="str">
+      <c r="Z17" s="15" t="str">
         <f>B17</f>
         <v>Hydrogen production - Decentralized Electrolysis</v>
       </c>
-      <c r="AA17" s="18" t="s">
+      <c r="AA17" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="AB17" s="18" t="s">
+      <c r="AB17" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="AC17" s="18" t="s">
+      <c r="AC17" s="15" t="s">
         <v>10</v>
       </c>
       <c r="AD17"/>
-      <c r="AE17" s="18" t="s">
+      <c r="AE17" s="15" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2394,331 +2394,331 @@
   </sheetPr>
   <dimension ref="A1:X10"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" style="18" customWidth="1"/>
-    <col min="2" max="2" width="29.28515625" style="18" customWidth="1"/>
-    <col min="3" max="5" width="12.85546875" style="18" customWidth="1"/>
-    <col min="6" max="8" width="8.85546875" style="18"/>
-    <col min="9" max="15" width="16.7109375" style="18" customWidth="1"/>
-    <col min="16" max="16" width="8.85546875" style="18"/>
-    <col min="17" max="17" width="11.7109375" style="18" customWidth="1"/>
-    <col min="18" max="18" width="11.7109375" style="18" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="21" style="18" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="8.85546875" style="18"/>
+    <col min="1" max="1" width="23.7109375" style="15" customWidth="1"/>
+    <col min="2" max="2" width="29.28515625" style="15" customWidth="1"/>
+    <col min="3" max="5" width="12.85546875" style="15" customWidth="1"/>
+    <col min="6" max="8" width="8.85546875" style="15"/>
+    <col min="9" max="15" width="16.7109375" style="15" customWidth="1"/>
+    <col min="16" max="16" width="8.85546875" style="15"/>
+    <col min="17" max="17" width="11.7109375" style="15" customWidth="1"/>
+    <col min="18" max="18" width="11.7109375" style="15" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="21" style="15" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="8.85546875" style="15"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="26" t="s">
         <v>104</v>
       </c>
-      <c r="B1" s="28"/>
+      <c r="B1" s="25"/>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="21" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="E3" s="26" t="s">
+      <c r="E3" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="Q3" s="26" t="s">
+      <c r="Q3" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="R3" s="25"/>
-      <c r="S3" s="25"/>
-      <c r="T3" s="25"/>
-      <c r="U3" s="25"/>
-      <c r="V3" s="25"/>
-      <c r="W3" s="25"/>
+      <c r="R3" s="22"/>
+      <c r="S3" s="22"/>
+      <c r="T3" s="22"/>
+      <c r="U3" s="22"/>
+      <c r="V3" s="22"/>
+      <c r="W3" s="22"/>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="38" t="s">
+      <c r="B4" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="C4" s="38" t="s">
+      <c r="C4" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="D4" s="38" t="s">
+      <c r="D4" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="E4" s="38" t="s">
+      <c r="E4" s="35" t="s">
         <v>103</v>
       </c>
-      <c r="F4" s="38" t="s">
+      <c r="F4" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="G4" s="38" t="s">
+      <c r="G4" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="H4" s="38" t="s">
+      <c r="H4" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="I4" s="38" t="s">
+      <c r="I4" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="J4" s="38" t="s">
+      <c r="J4" s="35" t="s">
         <v>102</v>
       </c>
-      <c r="K4" s="38" t="s">
+      <c r="K4" s="35" t="s">
         <v>101</v>
       </c>
-      <c r="L4" s="38" t="s">
+      <c r="L4" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="M4" s="38" t="s">
+      <c r="M4" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="N4" s="38" t="s">
+      <c r="N4" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="O4" s="38" t="s">
+      <c r="O4" s="35" t="s">
         <v>77</v>
       </c>
-      <c r="Q4" s="21" t="s">
+      <c r="Q4" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="R4" s="21" t="s">
+      <c r="R4" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="S4" s="21" t="s">
+      <c r="S4" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="T4" s="21" t="s">
+      <c r="T4" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="U4" s="21" t="s">
+      <c r="U4" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="V4" s="21" t="s">
+      <c r="V4" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="W4" s="21" t="s">
+      <c r="W4" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="X4" s="21" t="s">
+      <c r="X4" s="18" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:24" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="36" t="s">
+      <c r="A5" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="36" t="s">
+      <c r="C5" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="36" t="s">
+      <c r="D5" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="36" t="s">
+      <c r="E5" s="33" t="s">
         <v>100</v>
       </c>
-      <c r="F5" s="36"/>
-      <c r="G5" s="36" t="s">
+      <c r="F5" s="33"/>
+      <c r="G5" s="33" t="s">
         <v>99</v>
       </c>
-      <c r="H5" s="36" t="s">
+      <c r="H5" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="I5" s="36" t="s">
+      <c r="I5" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="J5" s="36" t="s">
+      <c r="J5" s="33" t="s">
         <v>98</v>
       </c>
-      <c r="K5" s="36" t="s">
+      <c r="K5" s="33" t="s">
         <v>97</v>
       </c>
-      <c r="L5" s="36" t="s">
+      <c r="L5" s="33" t="s">
         <v>96</v>
       </c>
-      <c r="M5" s="36" t="s">
+      <c r="M5" s="33" t="s">
         <v>95</v>
       </c>
-      <c r="N5" s="36" t="s">
+      <c r="N5" s="33" t="s">
         <v>94</v>
       </c>
-      <c r="O5" s="36" t="s">
+      <c r="O5" s="33" t="s">
         <v>93</v>
       </c>
-      <c r="Q5" s="35" t="s">
+      <c r="Q5" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="R5" s="35"/>
-      <c r="S5" s="35"/>
-      <c r="T5" s="35"/>
-      <c r="U5" s="35"/>
-      <c r="V5" s="35"/>
-      <c r="W5" s="35"/>
-      <c r="X5" s="35"/>
+      <c r="R5" s="32"/>
+      <c r="S5" s="32"/>
+      <c r="T5" s="32"/>
+      <c r="U5" s="32"/>
+      <c r="V5" s="32"/>
+      <c r="W5" s="32"/>
+      <c r="X5" s="32"/>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="B6" s="33"/>
-      <c r="C6" s="33"/>
-      <c r="D6" s="33"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="33" t="s">
+      <c r="B6" s="30"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="G6" s="33" t="s">
+      <c r="G6" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="H6" s="33"/>
-      <c r="I6" s="33" t="s">
+      <c r="H6" s="30"/>
+      <c r="I6" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="J6" s="33"/>
-      <c r="K6" s="33"/>
-      <c r="L6" s="33" t="s">
+      <c r="J6" s="30"/>
+      <c r="K6" s="30"/>
+      <c r="L6" s="30" t="s">
         <v>92</v>
       </c>
-      <c r="M6" s="33" t="s">
+      <c r="M6" s="30" t="s">
         <v>92</v>
       </c>
-      <c r="N6" s="33" t="s">
+      <c r="N6" s="30" t="s">
         <v>92</v>
       </c>
-      <c r="O6" s="33" t="s">
+      <c r="O6" s="30" t="s">
         <v>92</v>
       </c>
-      <c r="Q6" s="33" t="s">
+      <c r="Q6" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="R6" s="33"/>
-      <c r="S6" s="33"/>
-      <c r="T6" s="33"/>
-      <c r="U6" s="33"/>
-      <c r="V6" s="33"/>
-      <c r="W6" s="33"/>
-      <c r="X6" s="33"/>
+      <c r="R6" s="30"/>
+      <c r="S6" s="30"/>
+      <c r="T6" s="30"/>
+      <c r="U6" s="30"/>
+      <c r="V6" s="30"/>
+      <c r="W6" s="30"/>
+      <c r="X6" s="30"/>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A7" s="30" t="s">
+      <c r="A7" s="27" t="s">
         <v>91</v>
       </c>
-      <c r="B7" s="30"/>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="30"/>
-      <c r="I7" s="30"/>
-      <c r="J7" s="30"/>
-      <c r="K7" s="30"/>
-      <c r="L7" s="30"/>
-      <c r="M7" s="30"/>
-      <c r="N7" s="30"/>
-      <c r="O7" s="30"/>
-      <c r="Q7" s="30" t="str">
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="27"/>
+      <c r="J7" s="27"/>
+      <c r="K7" s="27"/>
+      <c r="L7" s="27"/>
+      <c r="M7" s="27"/>
+      <c r="N7" s="27"/>
+      <c r="O7" s="27"/>
+      <c r="Q7" s="27" t="str">
         <f>A7</f>
         <v>* Hydrogen liquefaction to HDL</v>
       </c>
-      <c r="R7" s="30"/>
-      <c r="S7" s="30"/>
-      <c r="T7" s="30"/>
-      <c r="U7" s="30"/>
-      <c r="V7" s="30"/>
-      <c r="W7" s="30"/>
-      <c r="X7" s="30"/>
+      <c r="R7" s="27"/>
+      <c r="S7" s="27"/>
+      <c r="T7" s="27"/>
+      <c r="U7" s="27"/>
+      <c r="V7" s="27"/>
+      <c r="W7" s="27"/>
+      <c r="X7" s="27"/>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="F8" s="18">
-        <v>2018</v>
-      </c>
-      <c r="G8" s="18">
+      <c r="F8" s="15">
+        <v>2019</v>
+      </c>
+      <c r="G8" s="15">
         <v>20</v>
       </c>
-      <c r="H8" s="18">
+      <c r="H8" s="15">
         <v>1</v>
       </c>
-      <c r="I8" s="18">
+      <c r="I8" s="15">
         <v>0.96</v>
       </c>
-      <c r="J8" s="18">
+      <c r="J8" s="15">
         <v>1</v>
       </c>
-      <c r="K8" s="18">
+      <c r="K8" s="15">
         <v>1</v>
       </c>
-      <c r="L8" s="39">
+      <c r="L8" s="36">
         <v>18.309289932000002</v>
       </c>
-      <c r="M8" s="39">
+      <c r="M8" s="36">
         <v>7.3237159728000005</v>
       </c>
-      <c r="N8" s="39">
+      <c r="N8" s="36">
         <v>1.2816502952400002</v>
       </c>
-      <c r="O8" s="39">
+      <c r="O8" s="36">
         <v>0.51266011809600009</v>
       </c>
-      <c r="Q8" s="18" t="s">
+      <c r="Q8" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="R8" s="18" t="str">
+      <c r="R8" s="15" t="str">
         <f>A8</f>
         <v>SH2GH2L_01</v>
       </c>
-      <c r="S8" s="18" t="str">
+      <c r="S8" s="15" t="str">
         <f>B8</f>
         <v>Hydrogen liquefaction</v>
       </c>
-      <c r="T8" s="18" t="s">
+      <c r="T8" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="U8" s="18" t="s">
+      <c r="U8" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="V8" s="18" t="s">
+      <c r="V8" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="X8" s="18" t="s">
+      <c r="X8" s="15" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="D9" s="18" t="s">
+      <c r="D9" s="15" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="E10" s="18" t="s">
+      <c r="E10" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="J10" s="39">
+      <c r="J10" s="36">
         <v>0.2195</v>
       </c>
-      <c r="K10" s="39">
+      <c r="K10" s="36">
         <v>0.17647058823529393</v>
       </c>
     </row>
@@ -2736,466 +2736,466 @@
   <dimension ref="A1:Z10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="E8" sqref="E8:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15" style="18" customWidth="1"/>
-    <col min="2" max="2" width="57.42578125" style="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="12.42578125" style="18" customWidth="1"/>
-    <col min="5" max="17" width="14.28515625" style="18" customWidth="1"/>
-    <col min="18" max="19" width="8.85546875" style="18"/>
-    <col min="20" max="20" width="11.7109375" style="18" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="56.42578125" style="18" bestFit="1" customWidth="1"/>
-    <col min="22" max="16384" width="8.85546875" style="18"/>
+    <col min="1" max="1" width="15" style="15" customWidth="1"/>
+    <col min="2" max="2" width="57.42578125" style="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.42578125" style="15" customWidth="1"/>
+    <col min="5" max="17" width="14.28515625" style="15" customWidth="1"/>
+    <col min="18" max="19" width="8.85546875" style="15"/>
+    <col min="20" max="20" width="11.7109375" style="15" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="56.42578125" style="15" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="8.85546875" style="15"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="26" t="s">
         <v>121</v>
       </c>
-      <c r="B1" s="28"/>
+      <c r="B1" s="25"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="21" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="D3" s="26" t="s">
+      <c r="D3" s="23" t="s">
         <v>120</v>
       </c>
-      <c r="S3" s="26" t="s">
+      <c r="S3" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="T3" s="25"/>
-      <c r="U3" s="25"/>
-      <c r="V3" s="25"/>
-      <c r="W3" s="25"/>
-      <c r="X3" s="25"/>
-      <c r="Y3" s="25"/>
+      <c r="T3" s="22"/>
+      <c r="U3" s="22"/>
+      <c r="V3" s="22"/>
+      <c r="W3" s="22"/>
+      <c r="X3" s="22"/>
+      <c r="Y3" s="22"/>
     </row>
     <row r="4" spans="1:26" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="38" t="s">
+      <c r="B4" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="C4" s="38" t="s">
+      <c r="C4" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="D4" s="38" t="s">
+      <c r="D4" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="E4" s="38" t="s">
+      <c r="E4" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="F4" s="38" t="s">
+      <c r="F4" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="G4" s="38" t="s">
+      <c r="G4" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="H4" s="38" t="s">
+      <c r="H4" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="I4" s="38" t="s">
+      <c r="I4" s="35" t="s">
         <v>102</v>
       </c>
-      <c r="J4" s="38" t="s">
+      <c r="J4" s="35" t="s">
         <v>101</v>
       </c>
-      <c r="K4" s="38" t="s">
+      <c r="K4" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="L4" s="38" t="s">
+      <c r="L4" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="M4" s="38" t="s">
+      <c r="M4" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="N4" s="38" t="s">
+      <c r="N4" s="35" t="s">
         <v>77</v>
       </c>
-      <c r="O4" s="38" t="s">
+      <c r="O4" s="35" t="s">
         <v>119</v>
       </c>
-      <c r="P4" s="38" t="s">
+      <c r="P4" s="35" t="s">
         <v>118</v>
       </c>
-      <c r="Q4" s="38" t="s">
+      <c r="Q4" s="35" t="s">
         <v>117</v>
       </c>
-      <c r="S4" s="21" t="s">
+      <c r="S4" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="T4" s="21" t="s">
+      <c r="T4" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="U4" s="21" t="s">
+      <c r="U4" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="V4" s="21" t="s">
+      <c r="V4" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="W4" s="21" t="s">
+      <c r="W4" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="X4" s="21" t="s">
+      <c r="X4" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="Y4" s="21" t="s">
+      <c r="Y4" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="Z4" s="21" t="s">
+      <c r="Z4" s="18" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="102.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="36" t="s">
+      <c r="A5" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="36" t="s">
+      <c r="C5" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="36" t="s">
+      <c r="D5" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="36" t="s">
+      <c r="E5" s="33" t="s">
         <v>99</v>
       </c>
-      <c r="F5" s="36" t="s">
+      <c r="F5" s="33" t="s">
         <v>99</v>
       </c>
-      <c r="G5" s="36" t="s">
+      <c r="G5" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="H5" s="36" t="s">
+      <c r="H5" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="I5" s="36" t="s">
+      <c r="I5" s="33" t="s">
         <v>98</v>
       </c>
-      <c r="J5" s="36" t="s">
+      <c r="J5" s="33" t="s">
         <v>97</v>
       </c>
-      <c r="K5" s="36" t="s">
+      <c r="K5" s="33" t="s">
         <v>96</v>
       </c>
-      <c r="L5" s="36" t="s">
+      <c r="L5" s="33" t="s">
         <v>95</v>
       </c>
-      <c r="M5" s="36" t="s">
+      <c r="M5" s="33" t="s">
         <v>94</v>
       </c>
-      <c r="N5" s="36" t="s">
+      <c r="N5" s="33" t="s">
         <v>93</v>
       </c>
-      <c r="O5" s="36" t="s">
+      <c r="O5" s="33" t="s">
         <v>116</v>
       </c>
-      <c r="P5" s="36" t="s">
+      <c r="P5" s="33" t="s">
         <v>115</v>
       </c>
-      <c r="Q5" s="36" t="s">
+      <c r="Q5" s="33" t="s">
         <v>114</v>
       </c>
-      <c r="S5" s="35" t="s">
+      <c r="S5" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="T5" s="35"/>
-      <c r="U5" s="35"/>
-      <c r="V5" s="35"/>
-      <c r="W5" s="35"/>
-      <c r="X5" s="35"/>
-      <c r="Y5" s="35"/>
-      <c r="Z5" s="35"/>
+      <c r="T5" s="32"/>
+      <c r="U5" s="32"/>
+      <c r="V5" s="32"/>
+      <c r="W5" s="32"/>
+      <c r="X5" s="32"/>
+      <c r="Y5" s="32"/>
+      <c r="Z5" s="32"/>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="B6" s="33"/>
-      <c r="C6" s="33"/>
-      <c r="D6" s="33"/>
-      <c r="E6" s="33" t="s">
+      <c r="B6" s="30"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="33" t="s">
+      <c r="F6" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="G6" s="33"/>
-      <c r="H6" s="33"/>
-      <c r="I6" s="33"/>
-      <c r="J6" s="33"/>
-      <c r="K6" s="33" t="s">
+      <c r="G6" s="30"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="30"/>
+      <c r="J6" s="30"/>
+      <c r="K6" s="30" t="s">
         <v>92</v>
       </c>
-      <c r="L6" s="33" t="s">
+      <c r="L6" s="30" t="s">
         <v>92</v>
       </c>
-      <c r="M6" s="33" t="s">
+      <c r="M6" s="30" t="s">
         <v>92</v>
       </c>
-      <c r="N6" s="33" t="s">
+      <c r="N6" s="30" t="s">
         <v>92</v>
       </c>
-      <c r="O6" s="33" t="s">
+      <c r="O6" s="30" t="s">
         <v>92</v>
       </c>
-      <c r="P6" s="33" t="s">
+      <c r="P6" s="30" t="s">
         <v>92</v>
       </c>
-      <c r="Q6" s="33" t="s">
+      <c r="Q6" s="30" t="s">
         <v>113</v>
       </c>
-      <c r="S6" s="33" t="s">
+      <c r="S6" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="T6" s="33"/>
-      <c r="U6" s="33"/>
-      <c r="V6" s="33"/>
-      <c r="W6" s="33"/>
-      <c r="X6" s="33"/>
-      <c r="Y6" s="33"/>
-      <c r="Z6" s="33"/>
+      <c r="T6" s="30"/>
+      <c r="U6" s="30"/>
+      <c r="V6" s="30"/>
+      <c r="W6" s="30"/>
+      <c r="X6" s="30"/>
+      <c r="Y6" s="30"/>
+      <c r="Z6" s="30"/>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A7" s="30" t="s">
+      <c r="A7" s="27" t="s">
         <v>112</v>
       </c>
-      <c r="B7" s="30"/>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="30"/>
-      <c r="I7" s="30"/>
-      <c r="J7" s="30"/>
-      <c r="K7" s="30"/>
-      <c r="L7" s="30"/>
-      <c r="M7" s="30"/>
-      <c r="N7" s="30"/>
-      <c r="O7" s="30"/>
-      <c r="P7" s="30"/>
-      <c r="Q7" s="30"/>
-      <c r="S7" s="30" t="str">
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="27"/>
+      <c r="J7" s="27"/>
+      <c r="K7" s="27"/>
+      <c r="L7" s="27"/>
+      <c r="M7" s="27"/>
+      <c r="N7" s="27"/>
+      <c r="O7" s="27"/>
+      <c r="P7" s="27"/>
+      <c r="Q7" s="27"/>
+      <c r="S7" s="27" t="str">
         <f>A7</f>
         <v>* Pipeline and road tanker distribution</v>
       </c>
-      <c r="T7" s="30"/>
-      <c r="U7" s="30"/>
-      <c r="V7" s="30"/>
-      <c r="W7" s="30"/>
-      <c r="X7" s="30"/>
-      <c r="Y7" s="30"/>
-      <c r="Z7" s="30"/>
+      <c r="T7" s="27"/>
+      <c r="U7" s="27"/>
+      <c r="V7" s="27"/>
+      <c r="W7" s="27"/>
+      <c r="X7" s="27"/>
+      <c r="Y7" s="27"/>
+      <c r="Z7" s="27"/>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="D8" s="18" t="s">
+      <c r="D8" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="18">
-        <v>2013</v>
-      </c>
-      <c r="F8" s="18">
+      <c r="E8" s="15">
+        <v>2019</v>
+      </c>
+      <c r="F8" s="15">
         <v>80</v>
       </c>
-      <c r="G8" s="18">
+      <c r="G8" s="15">
         <v>1</v>
       </c>
-      <c r="H8" s="18">
+      <c r="H8" s="15">
         <v>1</v>
       </c>
-      <c r="I8" s="18">
+      <c r="I8" s="15">
         <v>1</v>
       </c>
-      <c r="J8" s="18">
+      <c r="J8" s="15">
         <v>1</v>
       </c>
-      <c r="K8" s="19">
+      <c r="K8" s="16">
         <v>7.6759636785390413</v>
       </c>
-      <c r="L8" s="19">
+      <c r="L8" s="16">
         <v>7.6759636785390413</v>
       </c>
-      <c r="M8" s="19">
+      <c r="M8" s="16">
         <v>0.15351927357078055</v>
       </c>
-      <c r="N8" s="19">
+      <c r="N8" s="16">
         <v>0.15351927357078055</v>
       </c>
-      <c r="O8" s="19"/>
-      <c r="P8" s="19"/>
-      <c r="Q8" s="18">
+      <c r="O8" s="16"/>
+      <c r="P8" s="16"/>
+      <c r="Q8" s="15">
         <v>30</v>
       </c>
-      <c r="S8" s="18" t="s">
+      <c r="S8" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="T8" s="18" t="str">
-        <f>A8</f>
+      <c r="T8" s="15" t="str">
+        <f t="shared" ref="T8:U10" si="0">A8</f>
         <v>SH2GDEL_01</v>
       </c>
-      <c r="U8" s="18" t="str">
-        <f>B8</f>
+      <c r="U8" s="15" t="str">
+        <f t="shared" si="0"/>
         <v>Hydrogen Delivery - PIPELINE DISTRIBUTION HIGH-PRESSURE</v>
       </c>
-      <c r="V8" s="18" t="s">
+      <c r="V8" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="W8" s="18" t="s">
+      <c r="W8" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="X8" s="18" t="s">
+      <c r="X8" s="15" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="D9" s="18" t="s">
+      <c r="D9" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="E9" s="18">
-        <v>2013</v>
-      </c>
-      <c r="F9" s="18">
+      <c r="E9" s="15">
+        <v>2019</v>
+      </c>
+      <c r="F9" s="15">
         <v>15</v>
       </c>
-      <c r="G9" s="18">
+      <c r="G9" s="15">
         <v>1</v>
       </c>
-      <c r="H9" s="18">
+      <c r="H9" s="15">
         <v>1</v>
       </c>
-      <c r="I9" s="18">
+      <c r="I9" s="15">
         <v>1</v>
       </c>
-      <c r="J9" s="18">
+      <c r="J9" s="15">
         <v>1</v>
       </c>
-      <c r="K9" s="19">
+      <c r="K9" s="16">
         <v>4.9113986500408195</v>
       </c>
-      <c r="L9" s="19">
+      <c r="L9" s="16">
         <v>4.9113986500408195</v>
       </c>
-      <c r="M9" s="19">
+      <c r="M9" s="16">
         <v>1.2278496625102049</v>
       </c>
-      <c r="N9" s="19">
+      <c r="N9" s="16">
         <v>1.2278496625102049</v>
       </c>
-      <c r="O9" s="19">
+      <c r="O9" s="16">
         <v>0.55714989777013546</v>
       </c>
-      <c r="P9" s="19">
+      <c r="P9" s="16">
         <v>0.55714989777013546</v>
       </c>
-      <c r="T9" s="18" t="str">
-        <f>A9</f>
+      <c r="T9" s="15" t="str">
+        <f t="shared" si="0"/>
         <v>SH2LDEL_01</v>
       </c>
-      <c r="U9" s="18" t="str">
-        <f>B9</f>
+      <c r="U9" s="15" t="str">
+        <f t="shared" si="0"/>
         <v>Hydrogen Delivery - ROAD-TANKER DISTRIBUTION</v>
       </c>
-      <c r="V9" s="18" t="s">
+      <c r="V9" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="W9" s="18" t="s">
+      <c r="W9" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="X9" s="18" t="s">
+      <c r="X9" s="15" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A10" s="18" t="s">
+      <c r="A10" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="C10" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="D10" s="18" t="s">
+      <c r="D10" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="18">
-        <v>2013</v>
-      </c>
-      <c r="F10" s="18">
+      <c r="E10" s="15">
+        <v>2019</v>
+      </c>
+      <c r="F10" s="15">
         <v>80</v>
       </c>
-      <c r="G10" s="18">
+      <c r="G10" s="15">
         <v>1</v>
       </c>
-      <c r="H10" s="18">
+      <c r="H10" s="15">
         <v>1</v>
       </c>
-      <c r="I10" s="18">
+      <c r="I10" s="15">
         <v>1</v>
       </c>
-      <c r="J10" s="18">
+      <c r="J10" s="15">
         <v>1</v>
       </c>
-      <c r="K10" s="19">
+      <c r="K10" s="16">
         <v>2.506548</v>
       </c>
-      <c r="L10" s="19">
+      <c r="L10" s="16">
         <v>2.506548</v>
       </c>
-      <c r="M10" s="19">
+      <c r="M10" s="16">
         <v>5.0131000000000002E-2</v>
       </c>
-      <c r="N10" s="19">
+      <c r="N10" s="16">
         <v>5.0131000000000002E-2</v>
       </c>
-      <c r="O10" s="19"/>
-      <c r="P10" s="19"/>
-      <c r="Q10" s="18">
+      <c r="O10" s="16"/>
+      <c r="P10" s="16"/>
+      <c r="Q10" s="15">
         <v>30</v>
       </c>
-      <c r="T10" s="18" t="str">
-        <f>A10</f>
+      <c r="T10" s="15" t="str">
+        <f t="shared" si="0"/>
         <v>SH2GDEL_02</v>
       </c>
-      <c r="U10" s="18" t="str">
-        <f>B10</f>
+      <c r="U10" s="15" t="str">
+        <f t="shared" si="0"/>
         <v>Hydrogen Delivery - PIPELINE TRANSMISSION HIGH-PRESSURE</v>
       </c>
-      <c r="V10" s="18" t="s">
+      <c r="V10" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="W10" s="18" t="s">
+      <c r="W10" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="X10" s="18" t="s">
+      <c r="X10" s="15" t="s">
         <v>10</v>
       </c>
     </row>
@@ -3213,300 +3213,300 @@
   <dimension ref="A1:V8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="E7" sqref="E7:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" style="18" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" style="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="10.42578125" style="18" customWidth="1"/>
-    <col min="5" max="8" width="8.85546875" style="18"/>
-    <col min="9" max="9" width="14.42578125" style="18" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.28515625" style="18" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.7109375" style="18" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" style="15" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" style="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.42578125" style="15" customWidth="1"/>
+    <col min="5" max="8" width="8.85546875" style="15"/>
+    <col min="9" max="9" width="14.42578125" style="15" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.28515625" style="15" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" style="15" customWidth="1"/>
     <col min="12" max="12" width="6.42578125" customWidth="1"/>
-    <col min="13" max="13" width="11.42578125" style="18" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.85546875" style="18" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="23.28515625" style="18" bestFit="1" customWidth="1"/>
-    <col min="16" max="21" width="8.85546875" style="18"/>
+    <col min="13" max="13" width="11.42578125" style="15" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.85546875" style="15" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23.28515625" style="15" bestFit="1" customWidth="1"/>
+    <col min="16" max="21" width="8.85546875" style="15"/>
     <col min="22" max="22" width="2.7109375" customWidth="1"/>
-    <col min="23" max="16384" width="8.85546875" style="18"/>
+    <col min="23" max="16384" width="8.85546875" style="15"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="26" t="s">
         <v>134</v>
       </c>
-      <c r="B1" s="28"/>
+      <c r="B1" s="25"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="21" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="D3" s="26" t="s">
+      <c r="D3" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="M3" s="26" t="s">
+      <c r="M3" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="N3" s="25"/>
-      <c r="O3" s="25"/>
-      <c r="P3" s="25"/>
-      <c r="Q3" s="25"/>
-      <c r="R3" s="25"/>
-      <c r="S3" s="25"/>
+      <c r="N3" s="22"/>
+      <c r="O3" s="22"/>
+      <c r="P3" s="22"/>
+      <c r="Q3" s="22"/>
+      <c r="R3" s="22"/>
+      <c r="S3" s="22"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="38" t="s">
+      <c r="B4" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="C4" s="38" t="s">
+      <c r="C4" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="D4" s="38" t="s">
+      <c r="D4" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="E4" s="38" t="s">
+      <c r="E4" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="F4" s="38" t="s">
+      <c r="F4" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="G4" s="38" t="s">
+      <c r="G4" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="H4" s="38" t="s">
+      <c r="H4" s="35" t="s">
         <v>133</v>
       </c>
-      <c r="I4" s="38" t="s">
+      <c r="I4" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="J4" s="38" t="s">
+      <c r="J4" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="K4" s="38" t="s">
+      <c r="K4" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="M4" s="40" t="s">
+      <c r="M4" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="N4" s="40" t="s">
+      <c r="N4" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="O4" s="40" t="s">
+      <c r="O4" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="P4" s="40" t="s">
+      <c r="P4" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="Q4" s="40" t="s">
+      <c r="Q4" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="R4" s="40" t="s">
+      <c r="R4" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="S4" s="40" t="s">
+      <c r="S4" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="T4" s="40" t="s">
+      <c r="T4" s="37" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:20" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="36" t="s">
+      <c r="A5" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="36" t="s">
+      <c r="C5" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="36" t="s">
+      <c r="D5" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="36"/>
-      <c r="F5" s="36" t="s">
+      <c r="E5" s="33"/>
+      <c r="F5" s="33" t="s">
         <v>99</v>
       </c>
-      <c r="G5" s="36" t="s">
+      <c r="G5" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="H5" s="36" t="s">
+      <c r="H5" s="33" t="s">
         <v>132</v>
       </c>
-      <c r="I5" s="36" t="s">
+      <c r="I5" s="33" t="s">
         <v>131</v>
       </c>
-      <c r="J5" s="36" t="s">
+      <c r="J5" s="33" t="s">
         <v>130</v>
       </c>
-      <c r="K5" s="36" t="s">
+      <c r="K5" s="33" t="s">
         <v>129</v>
       </c>
-      <c r="M5" s="35" t="s">
+      <c r="M5" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="N5" s="35"/>
-      <c r="O5" s="35"/>
-      <c r="P5" s="35"/>
-      <c r="Q5" s="35"/>
-      <c r="R5" s="35"/>
-      <c r="S5" s="35"/>
-      <c r="T5" s="35"/>
+      <c r="N5" s="32"/>
+      <c r="O5" s="32"/>
+      <c r="P5" s="32"/>
+      <c r="Q5" s="32"/>
+      <c r="R5" s="32"/>
+      <c r="S5" s="32"/>
+      <c r="T5" s="32"/>
     </row>
     <row r="6" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="B6" s="33"/>
-      <c r="C6" s="33"/>
-      <c r="D6" s="33"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="33" t="s">
+      <c r="B6" s="30"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="G6" s="33"/>
-      <c r="H6" s="33"/>
-      <c r="I6" s="33" t="s">
+      <c r="G6" s="30"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="30" t="s">
         <v>92</v>
       </c>
-      <c r="J6" s="33" t="s">
+      <c r="J6" s="30" t="s">
         <v>92</v>
       </c>
-      <c r="K6" s="33" t="s">
+      <c r="K6" s="30" t="s">
         <v>128</v>
       </c>
-      <c r="M6" s="33" t="s">
+      <c r="M6" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="N6" s="33"/>
-      <c r="O6" s="33"/>
-      <c r="P6" s="33"/>
-      <c r="Q6" s="33"/>
-      <c r="R6" s="33"/>
-      <c r="S6" s="33"/>
-      <c r="T6" s="33"/>
+      <c r="N6" s="30"/>
+      <c r="O6" s="30"/>
+      <c r="P6" s="30"/>
+      <c r="Q6" s="30"/>
+      <c r="R6" s="30"/>
+      <c r="S6" s="30"/>
+      <c r="T6" s="30"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="15" t="s">
         <v>127</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="15" t="s">
         <v>126</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="D7" s="18" t="s">
+      <c r="D7" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="E7" s="18">
-        <v>2018</v>
-      </c>
-      <c r="F7" s="18">
+      <c r="E7" s="15">
+        <v>2019</v>
+      </c>
+      <c r="F7" s="15">
         <v>40</v>
       </c>
-      <c r="G7" s="18">
+      <c r="G7" s="15">
         <v>1</v>
       </c>
-      <c r="H7" s="18">
+      <c r="H7" s="15">
         <v>1</v>
       </c>
-      <c r="I7" s="39">
+      <c r="I7" s="36">
         <v>3.53</v>
       </c>
-      <c r="J7" s="39">
+      <c r="J7" s="36">
         <v>0.32078581007977441</v>
       </c>
-      <c r="K7" s="18">
+      <c r="K7" s="15">
         <v>1</v>
       </c>
-      <c r="M7" s="18" t="s">
+      <c r="M7" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="N7" s="18" t="str">
+      <c r="N7" s="15" t="str">
         <f>A7</f>
         <v>SH2GSTG_01</v>
       </c>
-      <c r="O7" s="18" t="str">
+      <c r="O7" s="15" t="str">
         <f>B7</f>
         <v>Hydrogen Storage - LARGE</v>
       </c>
-      <c r="P7" s="18" t="s">
+      <c r="P7" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="Q7" s="18" t="s">
+      <c r="Q7" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="R7" s="18" t="s">
+      <c r="R7" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="T7" s="18" t="s">
+      <c r="T7" s="15" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="15" t="s">
         <v>124</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="18" t="s">
+      <c r="D8" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="18">
-        <v>2018</v>
-      </c>
-      <c r="F8" s="18">
+      <c r="E8" s="15">
+        <v>2019</v>
+      </c>
+      <c r="F8" s="15">
         <v>40</v>
       </c>
-      <c r="G8" s="18">
+      <c r="G8" s="15">
         <v>1</v>
       </c>
-      <c r="H8" s="18">
+      <c r="H8" s="15">
         <v>1</v>
       </c>
-      <c r="I8" s="39">
+      <c r="I8" s="36">
         <v>23.67</v>
       </c>
-      <c r="J8" s="39">
+      <c r="J8" s="36">
         <v>0.93888529779446184</v>
       </c>
-      <c r="K8" s="18">
+      <c r="K8" s="15">
         <v>1</v>
       </c>
-      <c r="M8" s="18" t="s">
+      <c r="M8" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="N8" s="18" t="str">
+      <c r="N8" s="15" t="str">
         <f>A8</f>
         <v>SH2GSTG_02</v>
       </c>
-      <c r="O8" s="18" t="str">
+      <c r="O8" s="15" t="str">
         <f>B8</f>
         <v>Hydrogen Storage - SMALL</v>
       </c>
-      <c r="P8" s="18" t="s">
+      <c r="P8" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="Q8" s="18" t="s">
+      <c r="Q8" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="R8" s="18" t="s">
+      <c r="R8" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="T8" s="18" t="s">
+      <c r="T8" s="15" t="s">
         <v>122</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Remove PrimaryCG from an electrolyser
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_SUP_Hydrogen.xlsx
+++ b/SubRES_TMPL/SubRES_SUP_Hydrogen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A15BABD-44E3-424B-8FC9-8267CFE6931F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44132293-7DCC-4891-A420-552DBD99B71D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3233" yWindow="8002" windowWidth="20716" windowHeight="13276" activeTab="2" xr2:uid="{62F67F8D-DFD4-4ADE-8356-63F780461C4E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{62F67F8D-DFD4-4ADE-8356-63F780461C4E}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="2" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="134">
   <si>
     <t>UK TIMES</t>
   </si>
@@ -213,9 +213,6 @@
   </si>
   <si>
     <t>HYDROGEN decentralized production (H2PD)</t>
-  </si>
-  <si>
-    <t>NRGI</t>
   </si>
   <si>
     <t>DAYNITE</t>
@@ -1725,8 +1722,8 @@
   </sheetPr>
   <dimension ref="A2:AE17"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="S27" sqref="S27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1750,7 +1747,7 @@
   <sheetData>
     <row r="2" spans="1:31" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B2" s="25"/>
     </row>
@@ -1797,49 +1794,49 @@
         <v>45</v>
       </c>
       <c r="G5" s="35" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H5" s="35" t="s">
         <v>47</v>
       </c>
       <c r="I5" s="35" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J5" s="35" t="s">
         <v>43</v>
       </c>
       <c r="K5" s="35" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L5" s="35" t="s">
         <v>41</v>
       </c>
       <c r="M5" s="35" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="N5" s="35" t="s">
         <v>40</v>
       </c>
       <c r="O5" s="35" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="P5" s="35" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="Q5" s="35" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="R5" s="35" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="S5" s="35" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="T5" s="35" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="U5" s="35" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="X5" s="18" t="s">
         <v>35</v>
@@ -1881,37 +1878,37 @@
       </c>
       <c r="E6" s="33"/>
       <c r="F6" s="33" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G6" s="33" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H6" s="33" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I6" s="33" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J6" s="33" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K6" s="33" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L6" s="34" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M6" s="33"/>
       <c r="N6" s="33"/>
       <c r="O6" s="33"/>
       <c r="P6" s="34" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="Q6" s="33"/>
       <c r="R6" s="33"/>
       <c r="S6" s="33"/>
       <c r="T6" s="34" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="U6" s="33"/>
       <c r="X6" s="32" t="s">
@@ -1927,7 +1924,7 @@
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" s="30" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B7" s="30"/>
       <c r="C7" s="30"/>
@@ -1943,7 +1940,7 @@
       </c>
       <c r="H7" s="30"/>
       <c r="I7" s="30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J7" s="30"/>
       <c r="K7" s="30"/>
@@ -1960,7 +1957,7 @@
       <c r="R7" s="30"/>
       <c r="S7" s="30"/>
       <c r="T7" s="30" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="U7" s="30"/>
       <c r="X7" s="30" t="s">
@@ -1976,7 +1973,7 @@
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" s="27" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B8" s="28"/>
       <c r="C8" s="28"/>
@@ -2012,16 +2009,16 @@
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E9" s="15">
         <v>2019</v>
@@ -2082,9 +2079,6 @@
         <v>11</v>
       </c>
       <c r="AC9" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="AD9" s="15" t="s">
         <v>55</v>
       </c>
       <c r="AE9" s="15" t="s">
@@ -2394,8 +2388,8 @@
   </sheetPr>
   <dimension ref="A1:X10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2414,7 +2408,7 @@
   <sheetData>
     <row r="1" spans="1:24" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B1" s="25"/>
     </row>
@@ -2451,7 +2445,7 @@
         <v>48</v>
       </c>
       <c r="E4" s="35" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F4" s="35" t="s">
         <v>46</v>
@@ -2466,10 +2460,10 @@
         <v>44</v>
       </c>
       <c r="J4" s="35" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K4" s="35" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L4" s="35" t="s">
         <v>41</v>
@@ -2478,10 +2472,10 @@
         <v>40</v>
       </c>
       <c r="N4" s="35" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="O4" s="35" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="Q4" s="18" t="s">
         <v>35</v>
@@ -2522,35 +2516,35 @@
         <v>24</v>
       </c>
       <c r="E5" s="33" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F5" s="33"/>
       <c r="G5" s="33" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H5" s="33" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I5" s="33" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J5" s="33" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K5" s="33" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="L5" s="33" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="M5" s="33" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="N5" s="33" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="O5" s="33" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="Q5" s="32" t="s">
         <v>18</v>
@@ -2565,7 +2559,7 @@
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="30" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B6" s="30"/>
       <c r="C6" s="30"/>
@@ -2579,21 +2573,21 @@
       </c>
       <c r="H6" s="30"/>
       <c r="I6" s="30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J6" s="30"/>
       <c r="K6" s="30"/>
       <c r="L6" s="30" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="M6" s="30" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="N6" s="30" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="O6" s="30" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Q6" s="30" t="s">
         <v>18</v>
@@ -2608,7 +2602,7 @@
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="27" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B7" s="27"/>
       <c r="C7" s="27"/>
@@ -2638,13 +2632,13 @@
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F8" s="15">
         <v>2019</v>
@@ -2702,18 +2696,18 @@
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B9" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="D9" s="15" t="s">
         <v>87</v>
-      </c>
-      <c r="D9" s="15" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B10" s="15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J10" s="36">
         <v>0.2195</v>
@@ -2736,7 +2730,7 @@
   <dimension ref="A1:Z10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8:E10"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2753,7 +2747,7 @@
   <sheetData>
     <row r="1" spans="1:26" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B1" s="25"/>
     </row>
@@ -2764,7 +2758,7 @@
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="D3" s="23" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="S3" s="23" t="s">
         <v>51</v>
@@ -2802,10 +2796,10 @@
         <v>44</v>
       </c>
       <c r="I4" s="35" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J4" s="35" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K4" s="35" t="s">
         <v>41</v>
@@ -2814,19 +2808,19 @@
         <v>40</v>
       </c>
       <c r="M4" s="35" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="N4" s="35" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="O4" s="35" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="P4" s="35" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="Q4" s="35" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="S4" s="18" t="s">
         <v>35</v>
@@ -2867,43 +2861,43 @@
         <v>24</v>
       </c>
       <c r="E5" s="33" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F5" s="33" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G5" s="33" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H5" s="33" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I5" s="33" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J5" s="33" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K5" s="33" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L5" s="33" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="M5" s="33" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="N5" s="33" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="O5" s="33" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="P5" s="33" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="Q5" s="33" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="S5" s="32" t="s">
         <v>18</v>
@@ -2918,7 +2912,7 @@
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="30" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B6" s="30"/>
       <c r="C6" s="30"/>
@@ -2934,25 +2928,25 @@
       <c r="I6" s="30"/>
       <c r="J6" s="30"/>
       <c r="K6" s="30" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L6" s="30" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="M6" s="30" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="N6" s="30" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="O6" s="30" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="P6" s="30" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Q6" s="30" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="S6" s="30" t="s">
         <v>18</v>
@@ -2967,7 +2961,7 @@
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="27" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B7" s="27"/>
       <c r="C7" s="27"/>
@@ -2999,13 +2993,13 @@
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D8" s="15" t="s">
         <v>14</v>
@@ -3068,16 +3062,16 @@
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E9" s="15">
         <v>2019</v>
@@ -3135,13 +3129,13 @@
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D10" s="15" t="s">
         <v>14</v>
@@ -3212,8 +3206,8 @@
   </sheetPr>
   <dimension ref="A1:V8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7:E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3236,7 +3230,7 @@
   <sheetData>
     <row r="1" spans="1:20" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B1" s="25"/>
     </row>
@@ -3282,13 +3276,13 @@
         <v>47</v>
       </c>
       <c r="H4" s="35" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I4" s="35" t="s">
         <v>41</v>
       </c>
       <c r="J4" s="35" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K4" s="35" t="s">
         <v>44</v>
@@ -3333,22 +3327,22 @@
       </c>
       <c r="E5" s="33"/>
       <c r="F5" s="33" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G5" s="33" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H5" s="33" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I5" s="33" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J5" s="33" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K5" s="33" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="M5" s="32" t="s">
         <v>18</v>
@@ -3363,7 +3357,7 @@
     </row>
     <row r="6" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="30" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B6" s="30"/>
       <c r="C6" s="30"/>
@@ -3375,13 +3369,13 @@
       <c r="G6" s="30"/>
       <c r="H6" s="30"/>
       <c r="I6" s="30" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J6" s="30" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K6" s="30" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="M6" s="30" t="s">
         <v>18</v>
@@ -3396,16 +3390,16 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E7" s="15">
         <v>2019</v>
@@ -3429,7 +3423,7 @@
         <v>1</v>
       </c>
       <c r="M7" s="15" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="N7" s="15" t="str">
         <f>A7</f>
@@ -3449,15 +3443,15 @@
         <v>10</v>
       </c>
       <c r="T7" s="15" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C8" s="15" t="s">
         <v>14</v>
@@ -3487,7 +3481,7 @@
         <v>1</v>
       </c>
       <c r="M8" s="15" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="N8" s="15" t="str">
         <f>A8</f>
@@ -3507,7 +3501,7 @@
         <v>10</v>
       </c>
       <c r="T8" s="15" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>